<commit_message>
backtracking our optimised pòrtfolio with the benchmark
</commit_message>
<xml_diff>
--- a/portfolio-optimization/data/processed/etf_combined.xlsx
+++ b/portfolio-optimization/data/processed/etf_combined.xlsx
@@ -487,7 +487,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">WMVG LN </t>
+          <t>WMVG LN</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -502,7 +502,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">EMMV LN </t>
+          <t>EMMV LN</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -522,12 +522,12 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">PARAQPG LX </t>
+          <t>PARAQPG LX</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">GAMSUZA ID </t>
+          <t>GAMSUZA ID</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">CUKX LN </t>
+          <t>CUKX LN</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">VUKE LN </t>
+          <t>VUKE LN</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">VGSESIE ID </t>
+          <t>VGSESIE ID</t>
         </is>
       </c>
     </row>

</xml_diff>